<commit_message>
mz update doc assets
</commit_message>
<xml_diff>
--- a/docs/assets/datadict/Data Dictionary Documentation/template_dict_nhanes.xlsx
+++ b/docs/assets/datadict/Data Dictionary Documentation/template_dict_nhanes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itssastar-my.sharepoint.com/personal/tanmz-bii_bii_a-star_edu_sg/Documents/DAR/synData/copula-tabular/docs/assets/datadict/Data Dictionary Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C13D54E-FDC3-4854-B3B4-96497E6EF2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{0C13D54E-FDC3-4854-B3B4-96497E6EF2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC63DF05-E8B1-44FC-A283-B7AC3979CF46}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$78</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1215,11 +1228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1302,7 +1314,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1325,7 +1337,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1374,7 +1386,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1429,7 +1441,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>221</v>
       </c>
@@ -1455,7 +1467,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1481,7 +1493,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1507,7 +1519,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -1533,7 +1545,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1637,7 +1649,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
@@ -1663,7 +1675,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1801,7 +1813,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -1830,7 +1842,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
@@ -2200,7 +2212,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>43</v>
       </c>
@@ -2252,7 +2264,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>45</v>
       </c>
@@ -2330,7 +2342,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>48</v>
       </c>
@@ -2356,7 +2368,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>49</v>
       </c>
@@ -2486,7 +2498,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>54</v>
       </c>
@@ -2512,7 +2524,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>55</v>
       </c>
@@ -2564,7 +2576,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>57</v>
       </c>
@@ -2590,7 +2602,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>58</v>
       </c>
@@ -2668,7 +2680,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>61</v>
       </c>
@@ -2746,7 +2758,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>64</v>
       </c>
@@ -2772,7 +2784,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>65</v>
       </c>
@@ -2798,7 +2810,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>66</v>
       </c>
@@ -2850,7 +2862,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>68</v>
       </c>
@@ -2902,7 +2914,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>70</v>
       </c>
@@ -2954,7 +2966,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>72</v>
       </c>
@@ -2980,7 +2992,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>73</v>
       </c>
@@ -3084,7 +3096,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>77</v>
       </c>
@@ -3110,7 +3122,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>78</v>
       </c>
@@ -3136,7 +3148,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="42.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>79</v>
       </c>
@@ -3163,13 +3175,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J78" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="numeric"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J78" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>